<commit_message>
Update model & dataset
</commit_message>
<xml_diff>
--- a/run_this/generated_data_modifed_features.xlsx
+++ b/run_this/generated_data_modifed_features.xlsx
@@ -1398,7 +1398,7 @@
     <t>control232</t>
   </si>
   <si>
-    <t>21,1.2,62.339, 0.99</t>
+    <t>21, 1.2, 62.339, 0.99</t>
   </si>
   <si>
     <t>control233</t>
@@ -2701,7 +2701,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -2720,6 +2720,10 @@
     <font>
       <color theme="1"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <color theme="1"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="3">
@@ -2756,7 +2760,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -2767,6 +2771,9 @@
       <alignment horizontal="center" readingOrder="0" vertical="top"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -2987,7 +2994,8 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="2" width="7.63"/>
+    <col customWidth="1" min="1" max="1" width="10.88"/>
+    <col customWidth="1" min="2" max="2" width="7.63"/>
     <col customWidth="1" min="3" max="3" width="47.13"/>
     <col customWidth="1" min="4" max="4" width="30.0"/>
     <col customWidth="1" min="5" max="5" width="24.75"/>
@@ -3239,7 +3247,7 @@
       <c r="B21" s="3">
         <v>1.0</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C21" s="4" t="s">
         <v>47</v>
       </c>
     </row>
@@ -6556,7 +6564,7 @@
       <c r="B235" s="3">
         <v>0.0</v>
       </c>
-      <c r="C235" s="3" t="s">
+      <c r="C235" s="4" t="s">
         <v>460</v>
       </c>
     </row>
@@ -6822,7 +6830,7 @@
       <c r="A257" s="3" t="s">
         <v>503</v>
       </c>
-      <c r="B257" s="4">
+      <c r="B257" s="5">
         <v>1.0</v>
       </c>
       <c r="C257" s="3" t="s">
@@ -6842,7 +6850,7 @@
       <c r="A258" s="3" t="s">
         <v>505</v>
       </c>
-      <c r="B258" s="4">
+      <c r="B258" s="5">
         <v>1.0</v>
       </c>
       <c r="C258" s="3" t="s">
@@ -6862,7 +6870,7 @@
       <c r="A259" s="3" t="s">
         <v>507</v>
       </c>
-      <c r="B259" s="4">
+      <c r="B259" s="5">
         <v>1.0</v>
       </c>
       <c r="C259" s="3" t="s">
@@ -6882,7 +6890,7 @@
       <c r="A260" s="3" t="s">
         <v>509</v>
       </c>
-      <c r="B260" s="4">
+      <c r="B260" s="5">
         <v>1.0</v>
       </c>
       <c r="C260" s="3" t="s">
@@ -6902,7 +6910,7 @@
       <c r="A261" s="3" t="s">
         <v>511</v>
       </c>
-      <c r="B261" s="4">
+      <c r="B261" s="5">
         <v>1.0</v>
       </c>
       <c r="C261" s="3" t="s">
@@ -6922,7 +6930,7 @@
       <c r="A262" s="3" t="s">
         <v>513</v>
       </c>
-      <c r="B262" s="4">
+      <c r="B262" s="5">
         <v>1.0</v>
       </c>
       <c r="C262" s="3" t="s">
@@ -6942,7 +6950,7 @@
       <c r="A263" s="3" t="s">
         <v>515</v>
       </c>
-      <c r="B263" s="4">
+      <c r="B263" s="5">
         <v>1.0</v>
       </c>
       <c r="C263" s="3" t="s">
@@ -6962,7 +6970,7 @@
       <c r="A264" s="3" t="s">
         <v>517</v>
       </c>
-      <c r="B264" s="4">
+      <c r="B264" s="5">
         <v>1.0</v>
       </c>
       <c r="C264" s="3" t="s">
@@ -6982,7 +6990,7 @@
       <c r="A265" s="3" t="s">
         <v>519</v>
       </c>
-      <c r="B265" s="4">
+      <c r="B265" s="5">
         <v>1.0</v>
       </c>
       <c r="C265" s="3" t="s">
@@ -7002,7 +7010,7 @@
       <c r="A266" s="3" t="s">
         <v>521</v>
       </c>
-      <c r="B266" s="4">
+      <c r="B266" s="5">
         <v>1.0</v>
       </c>
       <c r="C266" s="3" t="s">
@@ -7022,7 +7030,7 @@
       <c r="A267" s="3" t="s">
         <v>523</v>
       </c>
-      <c r="B267" s="4">
+      <c r="B267" s="5">
         <v>1.0</v>
       </c>
       <c r="C267" s="3" t="s">
@@ -7042,7 +7050,7 @@
       <c r="A268" s="3" t="s">
         <v>525</v>
       </c>
-      <c r="B268" s="4">
+      <c r="B268" s="5">
         <v>1.0</v>
       </c>
       <c r="C268" s="3" t="s">
@@ -7062,7 +7070,7 @@
       <c r="A269" s="3" t="s">
         <v>527</v>
       </c>
-      <c r="B269" s="4">
+      <c r="B269" s="5">
         <v>1.0</v>
       </c>
       <c r="C269" s="3" t="s">
@@ -7082,7 +7090,7 @@
       <c r="A270" s="3" t="s">
         <v>529</v>
       </c>
-      <c r="B270" s="4">
+      <c r="B270" s="5">
         <v>1.0</v>
       </c>
       <c r="C270" s="3" t="s">
@@ -7102,7 +7110,7 @@
       <c r="A271" s="3" t="s">
         <v>531</v>
       </c>
-      <c r="B271" s="4">
+      <c r="B271" s="5">
         <v>1.0</v>
       </c>
       <c r="C271" s="3" t="s">
@@ -7122,7 +7130,7 @@
       <c r="A272" s="3" t="s">
         <v>533</v>
       </c>
-      <c r="B272" s="4">
+      <c r="B272" s="5">
         <v>1.0</v>
       </c>
       <c r="C272" s="3" t="s">
@@ -7142,7 +7150,7 @@
       <c r="A273" s="3" t="s">
         <v>535</v>
       </c>
-      <c r="B273" s="4">
+      <c r="B273" s="5">
         <v>1.0</v>
       </c>
       <c r="C273" s="3" t="s">
@@ -7162,7 +7170,7 @@
       <c r="A274" s="3" t="s">
         <v>537</v>
       </c>
-      <c r="B274" s="4">
+      <c r="B274" s="5">
         <v>1.0</v>
       </c>
       <c r="C274" s="3" t="s">
@@ -7182,7 +7190,7 @@
       <c r="A275" s="3" t="s">
         <v>539</v>
       </c>
-      <c r="B275" s="4">
+      <c r="B275" s="5">
         <v>1.0</v>
       </c>
       <c r="C275" s="3" t="s">
@@ -7202,7 +7210,7 @@
       <c r="A276" s="3" t="s">
         <v>541</v>
       </c>
-      <c r="B276" s="4">
+      <c r="B276" s="5">
         <v>1.0</v>
       </c>
       <c r="C276" s="3" t="s">
@@ -7222,7 +7230,7 @@
       <c r="A277" s="3" t="s">
         <v>543</v>
       </c>
-      <c r="B277" s="4">
+      <c r="B277" s="5">
         <v>1.0</v>
       </c>
       <c r="C277" s="3" t="s">
@@ -7242,7 +7250,7 @@
       <c r="A278" s="3" t="s">
         <v>545</v>
       </c>
-      <c r="B278" s="4">
+      <c r="B278" s="5">
         <v>1.0</v>
       </c>
       <c r="C278" s="3" t="s">
@@ -7262,7 +7270,7 @@
       <c r="A279" s="3" t="s">
         <v>547</v>
       </c>
-      <c r="B279" s="4">
+      <c r="B279" s="5">
         <v>1.0</v>
       </c>
       <c r="C279" s="3" t="s">
@@ -7282,7 +7290,7 @@
       <c r="A280" s="3" t="s">
         <v>549</v>
       </c>
-      <c r="B280" s="4">
+      <c r="B280" s="5">
         <v>1.0</v>
       </c>
       <c r="C280" s="3" t="s">
@@ -7302,7 +7310,7 @@
       <c r="A281" s="3" t="s">
         <v>551</v>
       </c>
-      <c r="B281" s="4">
+      <c r="B281" s="5">
         <v>1.0</v>
       </c>
       <c r="C281" s="3" t="s">
@@ -7322,7 +7330,7 @@
       <c r="A282" s="3" t="s">
         <v>553</v>
       </c>
-      <c r="B282" s="4">
+      <c r="B282" s="5">
         <v>1.0</v>
       </c>
       <c r="C282" s="3" t="s">
@@ -7342,7 +7350,7 @@
       <c r="A283" s="3" t="s">
         <v>555</v>
       </c>
-      <c r="B283" s="4">
+      <c r="B283" s="5">
         <v>1.0</v>
       </c>
       <c r="C283" s="3" t="s">
@@ -7362,7 +7370,7 @@
       <c r="A284" s="3" t="s">
         <v>557</v>
       </c>
-      <c r="B284" s="4">
+      <c r="B284" s="5">
         <v>1.0</v>
       </c>
       <c r="C284" s="3" t="s">
@@ -7382,7 +7390,7 @@
       <c r="A285" s="3" t="s">
         <v>559</v>
       </c>
-      <c r="B285" s="4">
+      <c r="B285" s="5">
         <v>1.0</v>
       </c>
       <c r="C285" s="3" t="s">
@@ -7402,7 +7410,7 @@
       <c r="A286" s="3" t="s">
         <v>561</v>
       </c>
-      <c r="B286" s="4">
+      <c r="B286" s="5">
         <v>1.0</v>
       </c>
       <c r="C286" s="3" t="s">
@@ -7422,7 +7430,7 @@
       <c r="A287" s="3" t="s">
         <v>563</v>
       </c>
-      <c r="B287" s="4">
+      <c r="B287" s="5">
         <v>1.0</v>
       </c>
       <c r="C287" s="3" t="s">
@@ -7442,7 +7450,7 @@
       <c r="A288" s="3" t="s">
         <v>565</v>
       </c>
-      <c r="B288" s="4">
+      <c r="B288" s="5">
         <v>1.0</v>
       </c>
       <c r="C288" s="3" t="s">
@@ -7462,7 +7470,7 @@
       <c r="A289" s="3" t="s">
         <v>567</v>
       </c>
-      <c r="B289" s="4">
+      <c r="B289" s="5">
         <v>1.0</v>
       </c>
       <c r="C289" s="3" t="s">
@@ -7482,7 +7490,7 @@
       <c r="A290" s="3" t="s">
         <v>569</v>
       </c>
-      <c r="B290" s="4">
+      <c r="B290" s="5">
         <v>1.0</v>
       </c>
       <c r="C290" s="3" t="s">
@@ -7502,7 +7510,7 @@
       <c r="A291" s="3" t="s">
         <v>571</v>
       </c>
-      <c r="B291" s="4">
+      <c r="B291" s="5">
         <v>1.0</v>
       </c>
       <c r="C291" s="3" t="s">
@@ -7539,7 +7547,7 @@
       <c r="A293" s="3" t="s">
         <v>575</v>
       </c>
-      <c r="B293" s="4">
+      <c r="B293" s="5">
         <v>1.0</v>
       </c>
       <c r="C293" s="3" t="s">
@@ -7556,7 +7564,7 @@
       <c r="A294" s="3" t="s">
         <v>577</v>
       </c>
-      <c r="B294" s="4">
+      <c r="B294" s="5">
         <v>1.0</v>
       </c>
       <c r="C294" s="3" t="s">
@@ -7573,7 +7581,7 @@
       <c r="A295" s="3" t="s">
         <v>579</v>
       </c>
-      <c r="B295" s="4">
+      <c r="B295" s="5">
         <v>1.0</v>
       </c>
       <c r="C295" s="3" t="s">
@@ -7590,7 +7598,7 @@
       <c r="A296" s="3" t="s">
         <v>581</v>
       </c>
-      <c r="B296" s="4">
+      <c r="B296" s="5">
         <v>1.0</v>
       </c>
       <c r="C296" s="3" t="s">
@@ -7607,7 +7615,7 @@
       <c r="A297" s="3" t="s">
         <v>583</v>
       </c>
-      <c r="B297" s="4">
+      <c r="B297" s="5">
         <v>1.0</v>
       </c>
       <c r="C297" s="3" t="s">
@@ -7624,7 +7632,7 @@
       <c r="A298" s="3" t="s">
         <v>585</v>
       </c>
-      <c r="B298" s="4">
+      <c r="B298" s="5">
         <v>1.0</v>
       </c>
       <c r="C298" s="3" t="s">
@@ -7641,7 +7649,7 @@
       <c r="A299" s="3" t="s">
         <v>587</v>
       </c>
-      <c r="B299" s="4">
+      <c r="B299" s="5">
         <v>1.0</v>
       </c>
       <c r="C299" s="3" t="s">
@@ -7658,7 +7666,7 @@
       <c r="A300" s="3" t="s">
         <v>589</v>
       </c>
-      <c r="B300" s="4">
+      <c r="B300" s="5">
         <v>1.0</v>
       </c>
       <c r="C300" s="3" t="s">
@@ -7675,7 +7683,7 @@
       <c r="A301" s="3" t="s">
         <v>591</v>
       </c>
-      <c r="B301" s="4">
+      <c r="B301" s="5">
         <v>1.0</v>
       </c>
       <c r="C301" s="3" t="s">
@@ -7832,7 +7840,7 @@
       <c r="A312" s="3" t="s">
         <v>613</v>
       </c>
-      <c r="B312" s="4">
+      <c r="B312" s="5">
         <v>1.0</v>
       </c>
       <c r="C312" s="3" t="s">
@@ -7846,7 +7854,7 @@
       <c r="A313" s="3" t="s">
         <v>615</v>
       </c>
-      <c r="B313" s="4">
+      <c r="B313" s="5">
         <v>1.0</v>
       </c>
       <c r="C313" s="3" t="s">
@@ -7860,7 +7868,7 @@
       <c r="A314" s="3" t="s">
         <v>617</v>
       </c>
-      <c r="B314" s="4">
+      <c r="B314" s="5">
         <v>1.0</v>
       </c>
       <c r="C314" s="3" t="s">
@@ -7874,7 +7882,7 @@
       <c r="A315" s="3" t="s">
         <v>619</v>
       </c>
-      <c r="B315" s="4">
+      <c r="B315" s="5">
         <v>1.0</v>
       </c>
       <c r="C315" s="3" t="s">
@@ -7888,7 +7896,7 @@
       <c r="A316" s="3" t="s">
         <v>621</v>
       </c>
-      <c r="B316" s="4">
+      <c r="B316" s="5">
         <v>1.0</v>
       </c>
       <c r="C316" s="3" t="s">
@@ -7902,7 +7910,7 @@
       <c r="A317" s="3" t="s">
         <v>623</v>
       </c>
-      <c r="B317" s="4">
+      <c r="B317" s="5">
         <v>1.0</v>
       </c>
       <c r="C317" s="3" t="s">
@@ -7916,7 +7924,7 @@
       <c r="A318" s="3" t="s">
         <v>625</v>
       </c>
-      <c r="B318" s="4">
+      <c r="B318" s="5">
         <v>1.0</v>
       </c>
       <c r="C318" s="3" t="s">
@@ -7930,7 +7938,7 @@
       <c r="A319" s="3" t="s">
         <v>627</v>
       </c>
-      <c r="B319" s="4">
+      <c r="B319" s="5">
         <v>1.0</v>
       </c>
       <c r="C319" s="3" t="s">
@@ -7944,7 +7952,7 @@
       <c r="A320" s="3" t="s">
         <v>629</v>
       </c>
-      <c r="B320" s="4">
+      <c r="B320" s="5">
         <v>1.0</v>
       </c>
       <c r="C320" s="3" t="s">
@@ -7958,7 +7966,7 @@
       <c r="A321" s="3" t="s">
         <v>631</v>
       </c>
-      <c r="B321" s="4">
+      <c r="B321" s="5">
         <v>1.0</v>
       </c>
       <c r="C321" s="3" t="s">
@@ -7972,7 +7980,7 @@
       <c r="A322" s="3" t="s">
         <v>633</v>
       </c>
-      <c r="B322" s="4">
+      <c r="B322" s="5">
         <v>1.0</v>
       </c>
       <c r="C322" s="3" t="s">
@@ -7986,7 +7994,7 @@
       <c r="A323" s="3" t="s">
         <v>635</v>
       </c>
-      <c r="B323" s="4">
+      <c r="B323" s="5">
         <v>1.0</v>
       </c>
       <c r="C323" s="3" t="s">
@@ -8000,7 +8008,7 @@
       <c r="A324" s="3" t="s">
         <v>637</v>
       </c>
-      <c r="B324" s="4">
+      <c r="B324" s="5">
         <v>1.0</v>
       </c>
       <c r="C324" s="3" t="s">
@@ -8014,7 +8022,7 @@
       <c r="A325" s="3" t="s">
         <v>639</v>
       </c>
-      <c r="B325" s="4">
+      <c r="B325" s="5">
         <v>1.0</v>
       </c>
       <c r="C325" s="3" t="s">
@@ -8028,7 +8036,7 @@
       <c r="A326" s="3" t="s">
         <v>641</v>
       </c>
-      <c r="B326" s="4">
+      <c r="B326" s="5">
         <v>1.0</v>
       </c>
       <c r="C326" s="3" t="s">
@@ -8042,7 +8050,7 @@
       <c r="A327" s="3" t="s">
         <v>643</v>
       </c>
-      <c r="B327" s="4">
+      <c r="B327" s="5">
         <v>1.0</v>
       </c>
       <c r="C327" s="3" t="s">
@@ -8056,7 +8064,7 @@
       <c r="A328" s="3" t="s">
         <v>645</v>
       </c>
-      <c r="B328" s="4">
+      <c r="B328" s="5">
         <v>1.0</v>
       </c>
       <c r="C328" s="3" t="s">
@@ -8070,7 +8078,7 @@
       <c r="A329" s="3" t="s">
         <v>647</v>
       </c>
-      <c r="B329" s="4">
+      <c r="B329" s="5">
         <v>1.0</v>
       </c>
       <c r="C329" s="3" t="s">
@@ -8084,7 +8092,7 @@
       <c r="A330" s="3" t="s">
         <v>649</v>
       </c>
-      <c r="B330" s="4">
+      <c r="B330" s="5">
         <v>1.0</v>
       </c>
       <c r="C330" s="3" t="s">
@@ -8098,7 +8106,7 @@
       <c r="A331" s="3" t="s">
         <v>651</v>
       </c>
-      <c r="B331" s="4">
+      <c r="B331" s="5">
         <v>1.0</v>
       </c>
       <c r="C331" s="3" t="s">
@@ -8112,7 +8120,7 @@
       <c r="A332" s="3" t="s">
         <v>653</v>
       </c>
-      <c r="B332" s="4">
+      <c r="B332" s="5">
         <v>1.0</v>
       </c>
       <c r="C332" s="3" t="s">
@@ -8126,7 +8134,7 @@
       <c r="A333" s="3" t="s">
         <v>655</v>
       </c>
-      <c r="B333" s="4">
+      <c r="B333" s="5">
         <v>1.0</v>
       </c>
       <c r="C333" s="3" t="s">
@@ -8140,7 +8148,7 @@
       <c r="A334" s="3" t="s">
         <v>657</v>
       </c>
-      <c r="B334" s="4">
+      <c r="B334" s="5">
         <v>1.0</v>
       </c>
       <c r="C334" s="3" t="s">
@@ -8154,7 +8162,7 @@
       <c r="A335" s="3" t="s">
         <v>659</v>
       </c>
-      <c r="B335" s="4">
+      <c r="B335" s="5">
         <v>1.0</v>
       </c>
       <c r="C335" s="3" t="s">
@@ -8168,7 +8176,7 @@
       <c r="A336" s="3" t="s">
         <v>661</v>
       </c>
-      <c r="B336" s="4">
+      <c r="B336" s="5">
         <v>1.0</v>
       </c>
       <c r="C336" s="3" t="s">
@@ -8182,7 +8190,7 @@
       <c r="A337" s="3" t="s">
         <v>663</v>
       </c>
-      <c r="B337" s="4">
+      <c r="B337" s="5">
         <v>1.0</v>
       </c>
       <c r="C337" s="3" t="s">
@@ -8196,7 +8204,7 @@
       <c r="A338" s="3" t="s">
         <v>665</v>
       </c>
-      <c r="B338" s="4">
+      <c r="B338" s="5">
         <v>1.0</v>
       </c>
       <c r="C338" s="3" t="s">
@@ -8210,7 +8218,7 @@
       <c r="A339" s="3" t="s">
         <v>667</v>
       </c>
-      <c r="B339" s="4">
+      <c r="B339" s="5">
         <v>1.0</v>
       </c>
       <c r="C339" s="3" t="s">
@@ -8224,7 +8232,7 @@
       <c r="A340" s="3" t="s">
         <v>669</v>
       </c>
-      <c r="B340" s="4">
+      <c r="B340" s="5">
         <v>1.0</v>
       </c>
       <c r="C340" s="3" t="s">
@@ -8238,7 +8246,7 @@
       <c r="A341" s="3" t="s">
         <v>671</v>
       </c>
-      <c r="B341" s="4">
+      <c r="B341" s="5">
         <v>1.0</v>
       </c>
       <c r="C341" s="3" t="s">
@@ -8252,7 +8260,7 @@
       <c r="A342" s="3" t="s">
         <v>673</v>
       </c>
-      <c r="B342" s="4">
+      <c r="B342" s="5">
         <v>1.0</v>
       </c>
       <c r="C342" s="3" t="s">
@@ -8266,7 +8274,7 @@
       <c r="A343" s="3" t="s">
         <v>675</v>
       </c>
-      <c r="B343" s="4">
+      <c r="B343" s="5">
         <v>1.0</v>
       </c>
       <c r="C343" s="3" t="s">
@@ -8280,7 +8288,7 @@
       <c r="A344" s="3" t="s">
         <v>677</v>
       </c>
-      <c r="B344" s="4">
+      <c r="B344" s="5">
         <v>1.0</v>
       </c>
       <c r="C344" s="3" t="s">
@@ -8294,7 +8302,7 @@
       <c r="A345" s="3" t="s">
         <v>679</v>
       </c>
-      <c r="B345" s="4">
+      <c r="B345" s="5">
         <v>1.0</v>
       </c>
       <c r="C345" s="3" t="s">
@@ -8308,7 +8316,7 @@
       <c r="A346" s="3" t="s">
         <v>681</v>
       </c>
-      <c r="B346" s="4">
+      <c r="B346" s="5">
         <v>1.0</v>
       </c>
       <c r="C346" s="3" t="s">
@@ -8322,7 +8330,7 @@
       <c r="A347" s="3" t="s">
         <v>683</v>
       </c>
-      <c r="B347" s="4">
+      <c r="B347" s="5">
         <v>1.0</v>
       </c>
       <c r="C347" s="3" t="s">
@@ -8336,7 +8344,7 @@
       <c r="A348" s="3" t="s">
         <v>685</v>
       </c>
-      <c r="B348" s="4">
+      <c r="B348" s="5">
         <v>1.0</v>
       </c>
       <c r="C348" s="3" t="s">
@@ -8350,7 +8358,7 @@
       <c r="A349" s="3" t="s">
         <v>687</v>
       </c>
-      <c r="B349" s="4">
+      <c r="B349" s="5">
         <v>1.0</v>
       </c>
       <c r="C349" s="3" t="s">
@@ -8364,7 +8372,7 @@
       <c r="A350" s="3" t="s">
         <v>689</v>
       </c>
-      <c r="B350" s="4">
+      <c r="B350" s="5">
         <v>1.0</v>
       </c>
       <c r="C350" s="3" t="s">
@@ -8378,7 +8386,7 @@
       <c r="A351" s="3" t="s">
         <v>691</v>
       </c>
-      <c r="B351" s="4">
+      <c r="B351" s="5">
         <v>1.0</v>
       </c>
       <c r="C351" s="3" t="s">
@@ -8710,7 +8718,7 @@
       <c r="B379" s="3">
         <v>1.0</v>
       </c>
-      <c r="C379" s="3" t="s">
+      <c r="C379" s="4" t="s">
         <v>748</v>
       </c>
       <c r="D379" s="3" t="s">

</xml_diff>